<commit_message>
histology - kidney GSH stats
</commit_message>
<xml_diff>
--- a/statistics/Spearmans-matrix-plots/results/Liver-Histology-QTL-Paper/correlations and p values.xlsx
+++ b/statistics/Spearmans-matrix-plots/results/Liver-Histology-QTL-Paper/correlations and p values.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beccagould/Rqtl2-Glutathione-Genetics/statistics/Spearmans-matrix-plots/results/Liver-Histology-QTL-Paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F88AAC92-5051-BE4D-8D53-E3ECC0BFD40C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F82C14B-E8D3-9243-B6CC-6978D0391778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12700" yWindow="500" windowWidth="16100" windowHeight="16320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14440" yWindow="500" windowWidth="14360" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Correlations" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="25">
   <si>
     <t>Body Weight (g)</t>
   </si>
@@ -69,6 +69,21 @@
   </si>
   <si>
     <t>Eh (mV)</t>
+  </si>
+  <si>
+    <t>Renal GSH (nmol/mg)</t>
+  </si>
+  <si>
+    <t>Renal GSSG (nmol/mg)</t>
+  </si>
+  <si>
+    <t>Renal Total Glutathione (nmol/mg)</t>
+  </si>
+  <si>
+    <t>Renal GSH/GSSG</t>
+  </si>
+  <si>
+    <t>Renal Eh (mV)</t>
   </si>
   <si>
     <t>Steatosis</t>
@@ -467,19 +482,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U21"/>
+  <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U12" sqref="U12"/>
+    <sheetView zoomScale="202" zoomScaleNormal="202" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" customWidth="1"/>
-    <col min="2" max="17" width="0" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="2" max="26" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -540,8 +555,23 @@
       <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -594,19 +624,34 @@
         <v>3.0827264318655338E-2</v>
       </c>
       <c r="R2">
+        <v>-0.15914263350394739</v>
+      </c>
+      <c r="S2">
+        <v>-0.1987952080157433</v>
+      </c>
+      <c r="T2">
+        <v>-0.17004951091132839</v>
+      </c>
+      <c r="U2">
+        <v>9.3642367604536841E-2</v>
+      </c>
+      <c r="V2">
+        <v>5.7621913608714949E-3</v>
+      </c>
+      <c r="W2">
         <v>0.30385755918504531</v>
       </c>
-      <c r="S2">
+      <c r="X2">
         <v>0.35220724993206082</v>
       </c>
-      <c r="T2">
+      <c r="Y2">
         <v>-3.4360057777691973E-2</v>
       </c>
-      <c r="U2">
+      <c r="Z2">
         <v>-0.16569625331770421</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -659,19 +704,34 @@
         <v>-0.18457486587394489</v>
       </c>
       <c r="R3">
+        <v>7.6701336629896436E-2</v>
+      </c>
+      <c r="S3">
+        <v>-7.5439112659934582E-2</v>
+      </c>
+      <c r="T3">
+        <v>7.2705617553235499E-2</v>
+      </c>
+      <c r="U3">
+        <v>0.12723834960772709</v>
+      </c>
+      <c r="V3">
+        <v>-0.12606319805709451</v>
+      </c>
+      <c r="W3">
         <v>-7.9564189795577764E-2</v>
       </c>
-      <c r="S3">
+      <c r="X3">
         <v>-0.11463999602447961</v>
       </c>
-      <c r="T3">
+      <c r="Y3">
         <v>-3.6168200582920771E-3</v>
       </c>
-      <c r="U3">
+      <c r="Z3">
         <v>8.609847288324797E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -724,19 +784,34 @@
         <v>-8.8157399015674251E-2</v>
       </c>
       <c r="R4">
+        <v>-1.4900734222068279E-2</v>
+      </c>
+      <c r="S4">
+        <v>-0.18945960269279691</v>
+      </c>
+      <c r="T4">
+        <v>-2.5244243256379591E-2</v>
+      </c>
+      <c r="U4">
+        <v>0.16454122266925769</v>
+      </c>
+      <c r="V4">
+        <v>-0.10943415367460819</v>
+      </c>
+      <c r="W4">
         <v>6.6451045374376322E-2</v>
       </c>
-      <c r="S4">
+      <c r="X4">
         <v>1.2500621365014109E-2</v>
       </c>
-      <c r="T4">
+      <c r="Y4">
         <v>-2.1745993546615331E-2</v>
       </c>
-      <c r="U4">
+      <c r="Z4">
         <v>5.3079754362879483E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -789,19 +864,34 @@
         <v>-0.14566008807970951</v>
       </c>
       <c r="R5">
+        <v>8.7173546483098593E-2</v>
+      </c>
+      <c r="S5">
+        <v>7.0725498647915622E-2</v>
+      </c>
+      <c r="T5">
+        <v>9.0169958854825219E-2</v>
+      </c>
+      <c r="U5">
+        <v>-6.3161198864957269E-3</v>
+      </c>
+      <c r="V5">
+        <v>-3.6304174276999043E-2</v>
+      </c>
+      <c r="W5">
         <v>-0.1205473437909399</v>
       </c>
-      <c r="S5">
+      <c r="X5">
         <v>-0.13020095206104229</v>
       </c>
-      <c r="T5">
+      <c r="Y5">
         <v>2.260006323422168E-2</v>
       </c>
-      <c r="U5">
+      <c r="Z5">
         <v>6.8933117246809505E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -854,19 +944,34 @@
         <v>-6.3175915870009133E-2</v>
       </c>
       <c r="R6">
+        <v>-5.3873463343310432E-2</v>
+      </c>
+      <c r="S6">
+        <v>-0.17243772572166399</v>
+      </c>
+      <c r="T6">
+        <v>-6.218769743763182E-2</v>
+      </c>
+      <c r="U6">
+        <v>0.12097313484515761</v>
+      </c>
+      <c r="V6">
+        <v>-5.0252814060719561E-2</v>
+      </c>
+      <c r="W6">
         <v>8.2097731650864744E-2</v>
       </c>
-      <c r="S6">
+      <c r="X6">
         <v>0.3162299321394767</v>
       </c>
-      <c r="T6">
+      <c r="Y6">
         <v>1.4227853350665809E-2</v>
       </c>
-      <c r="U6">
+      <c r="Z6">
         <v>-0.1426249368398512</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -919,19 +1024,34 @@
         <v>-0.30655920339547121</v>
       </c>
       <c r="R7">
+        <v>4.7859492808373108E-2</v>
+      </c>
+      <c r="S7">
+        <v>-0.1139161182689552</v>
+      </c>
+      <c r="T7">
+        <v>3.9214288042466849E-2</v>
+      </c>
+      <c r="U7">
+        <v>0.1514674888088493</v>
+      </c>
+      <c r="V7">
+        <v>-0.13567675115851341</v>
+      </c>
+      <c r="W7">
         <v>5.1239648367570237E-2</v>
       </c>
-      <c r="S7">
+      <c r="X7">
         <v>9.9804657263287411E-2</v>
       </c>
-      <c r="T7">
+      <c r="Y7">
         <v>-3.6891575219301448E-2</v>
       </c>
-      <c r="U7">
+      <c r="Z7">
         <v>7.1154598917007275E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -984,19 +1104,34 @@
         <v>0.22565311960212711</v>
       </c>
       <c r="R8">
+        <v>-0.26703819933352779</v>
+      </c>
+      <c r="S8">
+        <v>4.3407777102362148E-2</v>
+      </c>
+      <c r="T8">
+        <v>-0.25950882259308972</v>
+      </c>
+      <c r="U8">
+        <v>-0.25812402421917507</v>
+      </c>
+      <c r="V8">
+        <v>0.31057612022124992</v>
+      </c>
+      <c r="W8">
         <v>1.0486526171185151E-2</v>
       </c>
-      <c r="S8">
+      <c r="X8">
         <v>7.4654775452072095E-2</v>
       </c>
-      <c r="T8">
+      <c r="Y8">
         <v>0.1114740277005168</v>
       </c>
-      <c r="U8">
+      <c r="Z8">
         <v>3.7748140277124233E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1049,19 +1184,34 @@
         <v>-0.2344281867482331</v>
       </c>
       <c r="R9">
+        <v>0.18676056956539339</v>
+      </c>
+      <c r="S9">
+        <v>-0.113458032704001</v>
+      </c>
+      <c r="T9">
+        <v>0.17577560475222551</v>
+      </c>
+      <c r="U9">
+        <v>0.25626298649835222</v>
+      </c>
+      <c r="V9">
+        <v>-0.27235532620171371</v>
+      </c>
+      <c r="W9">
         <v>-1.158353626659009E-3</v>
       </c>
-      <c r="S9">
+      <c r="X9">
         <v>7.5436345184989179E-2</v>
       </c>
-      <c r="T9">
+      <c r="Y9">
         <v>5.8337078620655011E-3</v>
       </c>
-      <c r="U9">
+      <c r="Z9">
         <v>-8.3949156548683554E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1114,19 +1264,34 @@
         <v>0.24026591207120229</v>
       </c>
       <c r="R10">
+        <v>-0.21723424922483639</v>
+      </c>
+      <c r="S10">
+        <v>0.1145559819239759</v>
+      </c>
+      <c r="T10">
+        <v>-0.20483956194535549</v>
+      </c>
+      <c r="U10">
+        <v>-0.29251332652864692</v>
+      </c>
+      <c r="V10">
+        <v>0.3125259526675927</v>
+      </c>
+      <c r="W10">
         <v>-2.1071507143741341E-2</v>
       </c>
-      <c r="S10">
+      <c r="X10">
         <v>-1.879751371564839E-2</v>
       </c>
-      <c r="T10">
+      <c r="Y10">
         <v>8.6553036551480986E-2</v>
       </c>
-      <c r="U10">
+      <c r="Z10">
         <v>0.13339593336614869</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1179,19 +1344,34 @@
         <v>-5.046234955033508E-2</v>
       </c>
       <c r="R11">
+        <v>-0.1346009668532647</v>
+      </c>
+      <c r="S11">
+        <v>-0.2336853830170639</v>
+      </c>
+      <c r="T11">
+        <v>-0.14497018530038039</v>
+      </c>
+      <c r="U11">
+        <v>0.14629263202205139</v>
+      </c>
+      <c r="V11">
+        <v>-3.6755146001173557E-2</v>
+      </c>
+      <c r="W11">
         <v>0.271916462381046</v>
       </c>
-      <c r="S11">
+      <c r="X11">
         <v>0.38679120224656488</v>
       </c>
-      <c r="T11">
+      <c r="Y11">
         <v>-5.517518853436524E-2</v>
       </c>
-      <c r="U11">
+      <c r="Z11">
         <v>-0.16366604220934511</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1244,19 +1424,34 @@
         <v>-0.10014263669751571</v>
       </c>
       <c r="R12">
+        <v>-1.7399086627235189E-2</v>
+      </c>
+      <c r="S12">
+        <v>-0.1009415326077948</v>
+      </c>
+      <c r="T12">
+        <v>-1.9214214540032481E-2</v>
+      </c>
+      <c r="U12">
+        <v>8.4059482152619588E-2</v>
+      </c>
+      <c r="V12">
+        <v>-4.3035458895532869E-2</v>
+      </c>
+      <c r="W12">
         <v>9.3968595394097146E-2</v>
       </c>
-      <c r="S12">
+      <c r="X12">
         <v>0.1891757120402052</v>
       </c>
-      <c r="T12">
+      <c r="Y12">
         <v>-4.2327997857011468E-2</v>
       </c>
-      <c r="U12">
+      <c r="Z12">
         <v>-7.258097454693975E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1309,19 +1504,34 @@
         <v>-0.81000367201583534</v>
       </c>
       <c r="R13">
+        <v>0.1989854281876762</v>
+      </c>
+      <c r="S13">
+        <v>-5.8767532072354647E-2</v>
+      </c>
+      <c r="T13">
+        <v>0.1927129152134672</v>
+      </c>
+      <c r="U13">
+        <v>0.21850353892821031</v>
+      </c>
+      <c r="V13">
+        <v>-0.24626223738086889</v>
+      </c>
+      <c r="W13">
         <v>9.0220693819172953E-3</v>
       </c>
-      <c r="S13">
+      <c r="X13">
         <v>0.1049216673536626</v>
       </c>
-      <c r="T13">
+      <c r="Y13">
         <v>-0.11217561025408219</v>
       </c>
-      <c r="U13">
+      <c r="Z13">
         <v>0.1088620631300994</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1374,19 +1584,34 @@
         <v>-0.32563311478814472</v>
       </c>
       <c r="R14">
+        <v>0.15685567705699069</v>
+      </c>
+      <c r="S14">
+        <v>1.4344594804656779E-2</v>
+      </c>
+      <c r="T14">
+        <v>0.15441266558256031</v>
+      </c>
+      <c r="U14">
+        <v>0.1124841865156832</v>
+      </c>
+      <c r="V14">
+        <v>-0.14727896991419989</v>
+      </c>
+      <c r="W14">
         <v>9.1541445190814127E-2</v>
       </c>
-      <c r="S14">
+      <c r="X14">
         <v>8.372773728291262E-2</v>
       </c>
-      <c r="T14">
+      <c r="Y14">
         <v>-6.9759489095974278E-2</v>
       </c>
-      <c r="U14">
+      <c r="Z14">
         <v>8.5171046475752979E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -1439,19 +1664,34 @@
         <v>-0.79895923338159347</v>
       </c>
       <c r="R15">
+        <v>0.1993024726669089</v>
+      </c>
+      <c r="S15">
+        <v>-5.6022287995647492E-2</v>
+      </c>
+      <c r="T15">
+        <v>0.19319872577903641</v>
+      </c>
+      <c r="U15">
+        <v>0.21587697913196771</v>
+      </c>
+      <c r="V15">
+        <v>-0.24443189958346481</v>
+      </c>
+      <c r="W15">
         <v>1.315084045094911E-2</v>
       </c>
-      <c r="S15">
+      <c r="X15">
         <v>0.1047945923847269</v>
       </c>
-      <c r="T15">
+      <c r="Y15">
         <v>-0.1120421332637267</v>
       </c>
-      <c r="U15">
+      <c r="Z15">
         <v>0.10950304017067231</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -1504,19 +1744,34 @@
         <v>-0.65241325694864027</v>
       </c>
       <c r="R16">
+        <v>2.221124464434825E-2</v>
+      </c>
+      <c r="S16">
+        <v>-0.12579512592864561</v>
+      </c>
+      <c r="T16">
+        <v>1.4691643659693261E-2</v>
+      </c>
+      <c r="U16">
+        <v>0.14975872717669381</v>
+      </c>
+      <c r="V16">
+        <v>-0.12415684218508891</v>
+      </c>
+      <c r="W16">
         <v>-0.1756793028101333</v>
       </c>
-      <c r="S16">
+      <c r="X16">
         <v>8.4270015012030183E-3</v>
       </c>
-      <c r="T16">
+      <c r="Y16">
         <v>-3.5560981035050759E-2</v>
       </c>
-      <c r="U16">
+      <c r="Z16">
         <v>5.8617709486732811E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -1569,275 +1824,750 @@
         <v>1</v>
       </c>
       <c r="R17">
+        <v>-0.1536022281255304</v>
+      </c>
+      <c r="S17">
+        <v>0.1046137714338123</v>
+      </c>
+      <c r="T17">
+        <v>-0.1445993923683179</v>
+      </c>
+      <c r="U17">
+        <v>-0.2264377540702833</v>
+      </c>
+      <c r="V17">
+        <v>0.23764735707947779</v>
+      </c>
+      <c r="W17">
         <v>7.8432535250504212E-2</v>
       </c>
-      <c r="S17">
+      <c r="X17">
         <v>-9.1250923955127086E-2</v>
       </c>
-      <c r="T17">
+      <c r="Y17">
         <v>8.9742190518505113E-2</v>
       </c>
-      <c r="U17">
+      <c r="Z17">
         <v>-0.11251663227587171</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>-0.17004951091132839</v>
+      </c>
+      <c r="C18">
+        <v>7.2705617553235499E-2</v>
+      </c>
+      <c r="D18">
+        <v>-2.5244243256379591E-2</v>
+      </c>
+      <c r="E18">
+        <v>9.0169958854825219E-2</v>
+      </c>
+      <c r="F18">
+        <v>-6.218769743763182E-2</v>
+      </c>
+      <c r="G18">
+        <v>3.9214288042466849E-2</v>
+      </c>
+      <c r="H18">
+        <v>-0.25950882259308972</v>
+      </c>
+      <c r="I18">
+        <v>0.17577560475222551</v>
+      </c>
+      <c r="J18">
+        <v>-0.20483956194535549</v>
+      </c>
+      <c r="K18">
+        <v>-0.14497018530038039</v>
+      </c>
+      <c r="L18">
+        <v>-1.9214214540032481E-2</v>
+      </c>
+      <c r="M18">
+        <v>0.1927129152134672</v>
+      </c>
+      <c r="N18">
+        <v>0.15441266558256031</v>
+      </c>
+      <c r="O18">
+        <v>0.19319872577903641</v>
+      </c>
+      <c r="P18">
+        <v>1.4691643659693261E-2</v>
+      </c>
+      <c r="Q18">
+        <v>-0.1445993923683179</v>
+      </c>
+      <c r="R18">
+        <v>0.99799230306912934</v>
+      </c>
+      <c r="S18">
+        <v>0.3907547980756142</v>
+      </c>
+      <c r="T18">
+        <v>1</v>
+      </c>
+      <c r="U18">
+        <v>0.35853847072132328</v>
+      </c>
+      <c r="V18">
+        <v>-0.74123976727415963</v>
+      </c>
+      <c r="W18">
+        <v>1.292069828631894E-2</v>
+      </c>
+      <c r="X18">
+        <v>-0.17994427419890191</v>
+      </c>
+      <c r="Y18">
+        <v>-8.9832453696404389E-3</v>
+      </c>
+      <c r="Z18">
+        <v>9.9084499948084909E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B18">
-        <v>0.30385755918504531</v>
-      </c>
-      <c r="C18">
-        <v>-7.9564189795577764E-2</v>
-      </c>
-      <c r="D18">
-        <v>6.6451045374376322E-2</v>
-      </c>
-      <c r="E18">
-        <v>-0.1205473437909399</v>
-      </c>
-      <c r="F18">
-        <v>8.2097731650864744E-2</v>
-      </c>
-      <c r="G18">
-        <v>5.1239648367570237E-2</v>
-      </c>
-      <c r="H18">
-        <v>1.0486526171185151E-2</v>
-      </c>
-      <c r="I18">
-        <v>-1.158353626659009E-3</v>
-      </c>
-      <c r="J18">
-        <v>-2.1071507143741341E-2</v>
-      </c>
-      <c r="K18">
-        <v>0.271916462381046</v>
-      </c>
-      <c r="L18">
-        <v>9.3968595394097146E-2</v>
-      </c>
-      <c r="M18">
-        <v>9.0220693819172953E-3</v>
-      </c>
-      <c r="N18">
-        <v>9.1541445190814127E-2</v>
-      </c>
-      <c r="O18">
-        <v>1.315084045094911E-2</v>
-      </c>
-      <c r="P18">
-        <v>-0.1756793028101333</v>
-      </c>
-      <c r="Q18">
-        <v>7.8432535250504212E-2</v>
-      </c>
-      <c r="R18">
+      <c r="B19">
+        <v>-0.15914263350394739</v>
+      </c>
+      <c r="C19">
+        <v>7.6701336629896436E-2</v>
+      </c>
+      <c r="D19">
+        <v>-1.4900734222068279E-2</v>
+      </c>
+      <c r="E19">
+        <v>8.7173546483098593E-2</v>
+      </c>
+      <c r="F19">
+        <v>-5.3873463343310432E-2</v>
+      </c>
+      <c r="G19">
+        <v>4.7859492808373108E-2</v>
+      </c>
+      <c r="H19">
+        <v>-0.26703819933352779</v>
+      </c>
+      <c r="I19">
+        <v>0.18676056956539339</v>
+      </c>
+      <c r="J19">
+        <v>-0.21723424922483639</v>
+      </c>
+      <c r="K19">
+        <v>-0.1346009668532647</v>
+      </c>
+      <c r="L19">
+        <v>-1.7399086627235189E-2</v>
+      </c>
+      <c r="M19">
+        <v>0.1989854281876762</v>
+      </c>
+      <c r="N19">
+        <v>0.15685567705699069</v>
+      </c>
+      <c r="O19">
+        <v>0.1993024726669089</v>
+      </c>
+      <c r="P19">
+        <v>2.221124464434825E-2</v>
+      </c>
+      <c r="Q19">
+        <v>-0.1536022281255304</v>
+      </c>
+      <c r="R19">
         <v>1</v>
       </c>
-      <c r="S18">
-        <v>0.1160591934861377</v>
-      </c>
-      <c r="T18">
-        <v>6.7023185443333324E-3</v>
-      </c>
-      <c r="U18">
-        <v>-0.1086680041459397</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+      <c r="S19">
+        <v>0.34755932664176148</v>
+      </c>
+      <c r="T19">
+        <v>0.99799230306912934</v>
+      </c>
+      <c r="U19">
+        <v>0.40064986031409539</v>
+      </c>
+      <c r="V19">
+        <v>-0.77194894455009777</v>
+      </c>
+      <c r="W19">
+        <v>1.362471383069133E-2</v>
+      </c>
+      <c r="X19">
+        <v>-0.1836175583160114</v>
+      </c>
+      <c r="Y19">
+        <v>-5.9402445087790674E-3</v>
+      </c>
+      <c r="Z19">
+        <v>9.8555869551241168E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B19">
-        <v>0.35220724993206082</v>
-      </c>
-      <c r="C19">
-        <v>-0.11463999602447961</v>
-      </c>
-      <c r="D19">
-        <v>1.2500621365014109E-2</v>
-      </c>
-      <c r="E19">
-        <v>-0.13020095206104229</v>
-      </c>
-      <c r="F19">
-        <v>0.3162299321394767</v>
-      </c>
-      <c r="G19">
-        <v>9.9804657263287411E-2</v>
-      </c>
-      <c r="H19">
-        <v>7.4654775452072095E-2</v>
-      </c>
-      <c r="I19">
-        <v>7.5436345184989179E-2</v>
-      </c>
-      <c r="J19">
-        <v>-1.879751371564839E-2</v>
-      </c>
-      <c r="K19">
-        <v>0.38679120224656488</v>
-      </c>
-      <c r="L19">
-        <v>0.1891757120402052</v>
-      </c>
-      <c r="M19">
-        <v>0.1049216673536626</v>
-      </c>
-      <c r="N19">
-        <v>8.372773728291262E-2</v>
-      </c>
-      <c r="O19">
-        <v>0.1047945923847269</v>
-      </c>
-      <c r="P19">
-        <v>8.4270015012030183E-3</v>
-      </c>
-      <c r="Q19">
-        <v>-9.1250923955127086E-2</v>
-      </c>
-      <c r="R19">
-        <v>0.1160591934861377</v>
-      </c>
-      <c r="S19">
+      <c r="B20">
+        <v>-0.1987952080157433</v>
+      </c>
+      <c r="C20">
+        <v>-7.5439112659934582E-2</v>
+      </c>
+      <c r="D20">
+        <v>-0.18945960269279691</v>
+      </c>
+      <c r="E20">
+        <v>7.0725498647915622E-2</v>
+      </c>
+      <c r="F20">
+        <v>-0.17243772572166399</v>
+      </c>
+      <c r="G20">
+        <v>-0.1139161182689552</v>
+      </c>
+      <c r="H20">
+        <v>4.3407777102362148E-2</v>
+      </c>
+      <c r="I20">
+        <v>-0.113458032704001</v>
+      </c>
+      <c r="J20">
+        <v>0.1145559819239759</v>
+      </c>
+      <c r="K20">
+        <v>-0.2336853830170639</v>
+      </c>
+      <c r="L20">
+        <v>-0.1009415326077948</v>
+      </c>
+      <c r="M20">
+        <v>-5.8767532072354647E-2</v>
+      </c>
+      <c r="N20">
+        <v>1.4344594804656779E-2</v>
+      </c>
+      <c r="O20">
+        <v>-5.6022287995647492E-2</v>
+      </c>
+      <c r="P20">
+        <v>-0.12579512592864561</v>
+      </c>
+      <c r="Q20">
+        <v>0.1046137714338123</v>
+      </c>
+      <c r="R20">
+        <v>0.34755932664176148</v>
+      </c>
+      <c r="S20">
         <v>1</v>
       </c>
-      <c r="T19">
-        <v>-4.2990378092047921E-2</v>
-      </c>
-      <c r="U19">
-        <v>-0.15177152401124311</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20">
-        <v>-3.4360057777691973E-2</v>
-      </c>
-      <c r="C20">
-        <v>-3.6168200582920771E-3</v>
-      </c>
-      <c r="D20">
-        <v>-2.1745993546615331E-2</v>
-      </c>
-      <c r="E20">
-        <v>2.260006323422168E-2</v>
-      </c>
-      <c r="F20">
-        <v>1.4227853350665809E-2</v>
-      </c>
-      <c r="G20">
-        <v>-3.6891575219301448E-2</v>
-      </c>
-      <c r="H20">
-        <v>0.1114740277005168</v>
-      </c>
-      <c r="I20">
-        <v>5.8337078620655011E-3</v>
-      </c>
-      <c r="J20">
-        <v>8.6553036551480986E-2</v>
-      </c>
-      <c r="K20">
-        <v>-5.517518853436524E-2</v>
-      </c>
-      <c r="L20">
-        <v>-4.2327997857011468E-2</v>
-      </c>
-      <c r="M20">
-        <v>-0.11217561025408219</v>
-      </c>
-      <c r="N20">
-        <v>-6.9759489095974278E-2</v>
-      </c>
-      <c r="O20">
-        <v>-0.1120421332637267</v>
-      </c>
-      <c r="P20">
-        <v>-3.5560981035050759E-2</v>
-      </c>
-      <c r="Q20">
-        <v>8.9742190518505113E-2</v>
-      </c>
-      <c r="R20">
-        <v>6.7023185443333324E-3</v>
-      </c>
-      <c r="S20">
-        <v>-4.2990378092047921E-2</v>
-      </c>
       <c r="T20">
-        <v>1</v>
+        <v>0.3907547980756142</v>
       </c>
       <c r="U20">
-        <v>0.16552711929069419</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+        <v>-0.66528761220706267</v>
+      </c>
+      <c r="V20">
+        <v>0.26923624779972588</v>
+      </c>
+      <c r="W20">
+        <v>5.9336343606342899E-2</v>
+      </c>
+      <c r="X20">
+        <v>-2.101633168749064E-2</v>
+      </c>
+      <c r="Y20">
+        <v>-4.0516451382244252E-2</v>
+      </c>
+      <c r="Z20">
+        <v>2.0182990269542289E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B21">
+        <v>9.3642367604536841E-2</v>
+      </c>
+      <c r="C21">
+        <v>0.12723834960772709</v>
+      </c>
+      <c r="D21">
+        <v>0.16454122266925769</v>
+      </c>
+      <c r="E21">
+        <v>-6.3161198864957269E-3</v>
+      </c>
+      <c r="F21">
+        <v>0.12097313484515761</v>
+      </c>
+      <c r="G21">
+        <v>0.1514674888088493</v>
+      </c>
+      <c r="H21">
+        <v>-0.25812402421917507</v>
+      </c>
+      <c r="I21">
+        <v>0.25626298649835222</v>
+      </c>
+      <c r="J21">
+        <v>-0.29251332652864692</v>
+      </c>
+      <c r="K21">
+        <v>0.14629263202205139</v>
+      </c>
+      <c r="L21">
+        <v>8.4059482152619588E-2</v>
+      </c>
+      <c r="M21">
+        <v>0.21850353892821031</v>
+      </c>
+      <c r="N21">
+        <v>0.1124841865156832</v>
+      </c>
+      <c r="O21">
+        <v>0.21587697913196771</v>
+      </c>
+      <c r="P21">
+        <v>0.14975872717669381</v>
+      </c>
+      <c r="Q21">
+        <v>-0.2264377540702833</v>
+      </c>
+      <c r="R21">
+        <v>0.40064986031409539</v>
+      </c>
+      <c r="S21">
+        <v>-0.66528761220706267</v>
+      </c>
+      <c r="T21">
+        <v>0.35853847072132328</v>
+      </c>
+      <c r="U21">
+        <v>1</v>
+      </c>
+      <c r="V21">
+        <v>-0.8796624247185425</v>
+      </c>
+      <c r="W21">
+        <v>-1.5044246778764699E-2</v>
+      </c>
+      <c r="X21">
+        <v>-9.8691108920506365E-2</v>
+      </c>
+      <c r="Y21">
+        <v>3.117594219520951E-2</v>
+      </c>
+      <c r="Z21">
+        <v>4.3994639620673272E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>5.7621913608714949E-3</v>
+      </c>
+      <c r="C22">
+        <v>-0.12606319805709451</v>
+      </c>
+      <c r="D22">
+        <v>-0.10943415367460819</v>
+      </c>
+      <c r="E22">
+        <v>-3.6304174276999043E-2</v>
+      </c>
+      <c r="F22">
+        <v>-5.0252814060719561E-2</v>
+      </c>
+      <c r="G22">
+        <v>-0.13567675115851341</v>
+      </c>
+      <c r="H22">
+        <v>0.31057612022124992</v>
+      </c>
+      <c r="I22">
+        <v>-0.27235532620171371</v>
+      </c>
+      <c r="J22">
+        <v>0.3125259526675927</v>
+      </c>
+      <c r="K22">
+        <v>-3.6755146001173557E-2</v>
+      </c>
+      <c r="L22">
+        <v>-4.3035458895532869E-2</v>
+      </c>
+      <c r="M22">
+        <v>-0.24626223738086889</v>
+      </c>
+      <c r="N22">
+        <v>-0.14727896991419989</v>
+      </c>
+      <c r="O22">
+        <v>-0.24443189958346481</v>
+      </c>
+      <c r="P22">
+        <v>-0.12415684218508891</v>
+      </c>
+      <c r="Q22">
+        <v>0.23764735707947779</v>
+      </c>
+      <c r="R22">
+        <v>-0.77194894455009777</v>
+      </c>
+      <c r="S22">
+        <v>0.26923624779972588</v>
+      </c>
+      <c r="T22">
+        <v>-0.74123976727415963</v>
+      </c>
+      <c r="U22">
+        <v>-0.8796624247185425</v>
+      </c>
+      <c r="V22">
+        <v>1</v>
+      </c>
+      <c r="W22">
+        <v>-1.364749749168216E-2</v>
+      </c>
+      <c r="X22">
+        <v>0.15793773696776539</v>
+      </c>
+      <c r="Y22">
+        <v>-1.5595765667746319E-2</v>
+      </c>
+      <c r="Z22">
+        <v>-7.5878552598832139E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>0.30385755918504531</v>
+      </c>
+      <c r="C23">
+        <v>-7.9564189795577764E-2</v>
+      </c>
+      <c r="D23">
+        <v>6.6451045374376322E-2</v>
+      </c>
+      <c r="E23">
+        <v>-0.1205473437909399</v>
+      </c>
+      <c r="F23">
+        <v>8.2097731650864744E-2</v>
+      </c>
+      <c r="G23">
+        <v>5.1239648367570237E-2</v>
+      </c>
+      <c r="H23">
+        <v>1.0486526171185151E-2</v>
+      </c>
+      <c r="I23">
+        <v>-1.158353626659009E-3</v>
+      </c>
+      <c r="J23">
+        <v>-2.1071507143741341E-2</v>
+      </c>
+      <c r="K23">
+        <v>0.271916462381046</v>
+      </c>
+      <c r="L23">
+        <v>9.3968595394097146E-2</v>
+      </c>
+      <c r="M23">
+        <v>9.0220693819172953E-3</v>
+      </c>
+      <c r="N23">
+        <v>9.1541445190814127E-2</v>
+      </c>
+      <c r="O23">
+        <v>1.315084045094911E-2</v>
+      </c>
+      <c r="P23">
+        <v>-0.1756793028101333</v>
+      </c>
+      <c r="Q23">
+        <v>7.8432535250504212E-2</v>
+      </c>
+      <c r="R23">
+        <v>1.362471383069133E-2</v>
+      </c>
+      <c r="S23">
+        <v>5.9336343606342899E-2</v>
+      </c>
+      <c r="T23">
+        <v>1.292069828631894E-2</v>
+      </c>
+      <c r="U23">
+        <v>-1.5044246778764699E-2</v>
+      </c>
+      <c r="V23">
+        <v>-1.364749749168216E-2</v>
+      </c>
+      <c r="W23">
+        <v>1</v>
+      </c>
+      <c r="X23">
+        <v>0.1160591934861377</v>
+      </c>
+      <c r="Y23">
+        <v>6.7023185443333324E-3</v>
+      </c>
+      <c r="Z23">
+        <v>-0.1086680041459397</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>0.35220724993206082</v>
+      </c>
+      <c r="C24">
+        <v>-0.11463999602447961</v>
+      </c>
+      <c r="D24">
+        <v>1.2500621365014109E-2</v>
+      </c>
+      <c r="E24">
+        <v>-0.13020095206104229</v>
+      </c>
+      <c r="F24">
+        <v>0.3162299321394767</v>
+      </c>
+      <c r="G24">
+        <v>9.9804657263287411E-2</v>
+      </c>
+      <c r="H24">
+        <v>7.4654775452072095E-2</v>
+      </c>
+      <c r="I24">
+        <v>7.5436345184989179E-2</v>
+      </c>
+      <c r="J24">
+        <v>-1.879751371564839E-2</v>
+      </c>
+      <c r="K24">
+        <v>0.38679120224656488</v>
+      </c>
+      <c r="L24">
+        <v>0.1891757120402052</v>
+      </c>
+      <c r="M24">
+        <v>0.1049216673536626</v>
+      </c>
+      <c r="N24">
+        <v>8.372773728291262E-2</v>
+      </c>
+      <c r="O24">
+        <v>0.1047945923847269</v>
+      </c>
+      <c r="P24">
+        <v>8.4270015012030183E-3</v>
+      </c>
+      <c r="Q24">
+        <v>-9.1250923955127086E-2</v>
+      </c>
+      <c r="R24">
+        <v>-0.1836175583160114</v>
+      </c>
+      <c r="S24">
+        <v>-2.101633168749064E-2</v>
+      </c>
+      <c r="T24">
+        <v>-0.17994427419890191</v>
+      </c>
+      <c r="U24">
+        <v>-9.8691108920506365E-2</v>
+      </c>
+      <c r="V24">
+        <v>0.15793773696776539</v>
+      </c>
+      <c r="W24">
+        <v>0.1160591934861377</v>
+      </c>
+      <c r="X24">
+        <v>1</v>
+      </c>
+      <c r="Y24">
+        <v>-4.2990378092047921E-2</v>
+      </c>
+      <c r="Z24">
+        <v>-0.15177152401124311</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>-3.4360057777691973E-2</v>
+      </c>
+      <c r="C25">
+        <v>-3.6168200582920771E-3</v>
+      </c>
+      <c r="D25">
+        <v>-2.1745993546615331E-2</v>
+      </c>
+      <c r="E25">
+        <v>2.260006323422168E-2</v>
+      </c>
+      <c r="F25">
+        <v>1.4227853350665809E-2</v>
+      </c>
+      <c r="G25">
+        <v>-3.6891575219301448E-2</v>
+      </c>
+      <c r="H25">
+        <v>0.1114740277005168</v>
+      </c>
+      <c r="I25">
+        <v>5.8337078620655011E-3</v>
+      </c>
+      <c r="J25">
+        <v>8.6553036551480986E-2</v>
+      </c>
+      <c r="K25">
+        <v>-5.517518853436524E-2</v>
+      </c>
+      <c r="L25">
+        <v>-4.2327997857011468E-2</v>
+      </c>
+      <c r="M25">
+        <v>-0.11217561025408219</v>
+      </c>
+      <c r="N25">
+        <v>-6.9759489095974278E-2</v>
+      </c>
+      <c r="O25">
+        <v>-0.1120421332637267</v>
+      </c>
+      <c r="P25">
+        <v>-3.5560981035050759E-2</v>
+      </c>
+      <c r="Q25">
+        <v>8.9742190518505113E-2</v>
+      </c>
+      <c r="R25">
+        <v>-5.9402445087790674E-3</v>
+      </c>
+      <c r="S25">
+        <v>-4.0516451382244252E-2</v>
+      </c>
+      <c r="T25">
+        <v>-8.9832453696404389E-3</v>
+      </c>
+      <c r="U25">
+        <v>3.117594219520951E-2</v>
+      </c>
+      <c r="V25">
+        <v>-1.5595765667746319E-2</v>
+      </c>
+      <c r="W25">
+        <v>6.7023185443333324E-3</v>
+      </c>
+      <c r="X25">
+        <v>-4.2990378092047921E-2</v>
+      </c>
+      <c r="Y25">
+        <v>1</v>
+      </c>
+      <c r="Z25">
+        <v>0.16552711929069419</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26">
         <v>-0.16569625331770421</v>
       </c>
-      <c r="C21">
+      <c r="C26">
         <v>8.609847288324797E-2</v>
       </c>
-      <c r="D21">
+      <c r="D26">
         <v>5.3079754362879483E-2</v>
       </c>
-      <c r="E21">
+      <c r="E26">
         <v>6.8933117246809505E-2</v>
       </c>
-      <c r="F21">
+      <c r="F26">
         <v>-0.1426249368398512</v>
       </c>
-      <c r="G21">
+      <c r="G26">
         <v>7.1154598917007275E-2</v>
       </c>
-      <c r="H21">
+      <c r="H26">
         <v>3.7748140277124233E-2</v>
       </c>
-      <c r="I21">
+      <c r="I26">
         <v>-8.3949156548683554E-2</v>
       </c>
-      <c r="J21">
+      <c r="J26">
         <v>0.13339593336614869</v>
       </c>
-      <c r="K21">
+      <c r="K26">
         <v>-0.16366604220934511</v>
       </c>
-      <c r="L21">
+      <c r="L26">
         <v>-7.258097454693975E-2</v>
       </c>
-      <c r="M21">
+      <c r="M26">
         <v>0.1088620631300994</v>
       </c>
-      <c r="N21">
+      <c r="N26">
         <v>8.5171046475752979E-2</v>
       </c>
-      <c r="O21">
+      <c r="O26">
         <v>0.10950304017067231</v>
       </c>
-      <c r="P21">
+      <c r="P26">
         <v>5.8617709486732811E-2</v>
       </c>
-      <c r="Q21">
+      <c r="Q26">
         <v>-0.11251663227587171</v>
       </c>
-      <c r="R21">
+      <c r="R26">
+        <v>9.8555869551241168E-2</v>
+      </c>
+      <c r="S26">
+        <v>2.0182990269542289E-2</v>
+      </c>
+      <c r="T26">
+        <v>9.9084499948084909E-2</v>
+      </c>
+      <c r="U26">
+        <v>4.3994639620673272E-2</v>
+      </c>
+      <c r="V26">
+        <v>-7.5878552598832139E-2</v>
+      </c>
+      <c r="W26">
         <v>-0.1086680041459397</v>
       </c>
-      <c r="S21">
+      <c r="X26">
         <v>-0.15177152401124311</v>
       </c>
-      <c r="T21">
+      <c r="Y26">
         <v>0.16552711929069419</v>
       </c>
-      <c r="U21">
+      <c r="Z26">
         <v>1</v>
       </c>
     </row>
@@ -1848,19 +2578,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:U21"/>
+  <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T12" sqref="T12"/>
+    <sheetView tabSelected="1" zoomScale="183" zoomScaleNormal="183" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.1640625" customWidth="1"/>
-    <col min="2" max="17" width="0" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="2" max="5" width="8.83203125" hidden="1" customWidth="1"/>
+    <col min="6" max="26" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1921,8 +2652,23 @@
       <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1972,19 +2718,34 @@
         <v>0.56767360353229956</v>
       </c>
       <c r="R2">
+        <v>3.0354181976899319E-3</v>
+      </c>
+      <c r="S2">
+        <v>2.0223074938652269E-4</v>
+      </c>
+      <c r="T2">
+        <v>1.5234122749419039E-3</v>
+      </c>
+      <c r="U2">
+        <v>8.2416198412975872E-2</v>
+      </c>
+      <c r="V2">
+        <v>0.91507425958794109</v>
+      </c>
+      <c r="W2">
         <v>7.9940312147641635E-9</v>
       </c>
-      <c r="S2">
+      <c r="X2">
         <v>1.5294654431841082E-11</v>
       </c>
-      <c r="T2">
+      <c r="Y2">
         <v>0.52351544353247403</v>
       </c>
-      <c r="U2">
+      <c r="Z2">
         <v>1.9855965758854839E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2034,19 +2795,34 @@
         <v>6.0266883941850757E-4</v>
       </c>
       <c r="R3">
+        <v>0.15757841399975231</v>
+      </c>
+      <c r="S3">
+        <v>0.16454747370130329</v>
+      </c>
+      <c r="T3">
+        <v>0.18042785785380319</v>
+      </c>
+      <c r="U3">
+        <v>1.8746157816013301E-2</v>
+      </c>
+      <c r="V3">
+        <v>1.9877306910976111E-2</v>
+      </c>
+      <c r="W3">
         <v>0.14201147788876761</v>
       </c>
-      <c r="S3">
+      <c r="X3">
         <v>3.4065538884172852E-2</v>
       </c>
-      <c r="T3">
+      <c r="Y3">
         <v>0.94678857817506135</v>
       </c>
-      <c r="U3">
+      <c r="Z3">
         <v>0.11197844587601311</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -2096,19 +2872,34 @@
         <v>0.1041372592434666</v>
       </c>
       <c r="R4">
+        <v>0.78426958913470668</v>
+      </c>
+      <c r="S4">
+        <v>4.4397665061057801E-4</v>
+      </c>
+      <c r="T4">
+        <v>0.64276199117829647</v>
+      </c>
+      <c r="U4">
+        <v>2.3377543571192478E-3</v>
+      </c>
+      <c r="V4">
+        <v>4.374825080269451E-2</v>
+      </c>
+      <c r="W4">
         <v>0.22097305700749681</v>
       </c>
-      <c r="S4">
+      <c r="X4">
         <v>0.81809164219173258</v>
       </c>
-      <c r="T4">
+      <c r="Y4">
         <v>0.68861967565947912</v>
       </c>
-      <c r="U4">
+      <c r="Z4">
         <v>0.32843522518317952</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -2158,19 +2949,34 @@
         <v>7.1385455671173492E-3</v>
       </c>
       <c r="R5">
+        <v>0.1091206331934611</v>
+      </c>
+      <c r="S5">
+        <v>0.19393981618976919</v>
+      </c>
+      <c r="T5">
+        <v>9.7428371433279981E-2</v>
+      </c>
+      <c r="U5">
+        <v>0.90776054857610999</v>
+      </c>
+      <c r="V5">
+        <v>0.50529511325417786</v>
+      </c>
+      <c r="W5">
         <v>2.623544624303786E-2</v>
       </c>
-      <c r="S5">
+      <c r="X5">
         <v>1.6297710362367161E-2</v>
       </c>
-      <c r="T5">
+      <c r="Y5">
         <v>0.67751416115935603</v>
       </c>
-      <c r="U5">
+      <c r="Z5">
         <v>0.20483667461513291</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -2220,19 +3026,34 @@
         <v>0.24117354301873381</v>
       </c>
       <c r="R6">
+        <v>0.31840143037489699</v>
+      </c>
+      <c r="S6">
+        <v>1.3027048439997471E-3</v>
+      </c>
+      <c r="T6">
+        <v>0.2493176011176246</v>
+      </c>
+      <c r="U6">
+        <v>2.4634913323675619E-2</v>
+      </c>
+      <c r="V6">
+        <v>0.35205785424784031</v>
+      </c>
+      <c r="W6">
         <v>0.12747029830778309</v>
       </c>
-      <c r="S6">
+      <c r="X6">
         <v>1.787699543953636E-9</v>
       </c>
-      <c r="T6">
+      <c r="Y6">
         <v>0.79170857727050126</v>
       </c>
-      <c r="U6">
+      <c r="Z6">
         <v>7.884574595334648E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -2282,19 +3103,34 @@
         <v>1.2414655969905651E-8</v>
       </c>
       <c r="R7">
+        <v>0.38543230182208182</v>
+      </c>
+      <c r="S7">
+        <v>3.8318701261943033E-2</v>
+      </c>
+      <c r="T7">
+        <v>0.47707431191177768</v>
+      </c>
+      <c r="U7">
+        <v>5.7583542686199252E-3</v>
+      </c>
+      <c r="V7">
+        <v>1.3491751282044721E-2</v>
+      </c>
+      <c r="W7">
         <v>0.35272965857318411</v>
       </c>
-      <c r="S7">
+      <c r="X7">
         <v>6.9762797552677336E-2</v>
       </c>
-      <c r="T7">
+      <c r="Y7">
         <v>0.50292835471340336</v>
       </c>
-      <c r="U7">
+      <c r="Z7">
         <v>0.19660505964039571</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -2344,19 +3180,34 @@
         <v>3.5169104668941742E-5</v>
       </c>
       <c r="R8">
+        <v>8.5552872164385008E-7</v>
+      </c>
+      <c r="S8">
+        <v>0.43191446071589651</v>
+      </c>
+      <c r="T8">
+        <v>1.7666464176002709E-6</v>
+      </c>
+      <c r="U8">
+        <v>2.0138057497121049E-6</v>
+      </c>
+      <c r="V8">
+        <v>8.2320865679719191E-9</v>
+      </c>
+      <c r="W8">
         <v>0.84948185369671969</v>
       </c>
-      <c r="S8">
+      <c r="X8">
         <v>0.1760831168296795</v>
       </c>
-      <c r="T8">
+      <c r="Y8">
         <v>4.2688932613786923E-2</v>
       </c>
-      <c r="U8">
+      <c r="Z8">
         <v>0.49437267771767651</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -2406,19 +3257,34 @@
         <v>1.4996461267013931E-5</v>
       </c>
       <c r="R9">
+        <v>6.1382250129948801E-4</v>
+      </c>
+      <c r="S9">
+        <v>3.8516460401481822E-2</v>
+      </c>
+      <c r="T9">
+        <v>1.278985204954397E-3</v>
+      </c>
+      <c r="U9">
+        <v>2.156992431334714E-6</v>
+      </c>
+      <c r="V9">
+        <v>4.4866565440671019E-7</v>
+      </c>
+      <c r="W9">
         <v>0.98317360079058647</v>
       </c>
-      <c r="S9">
+      <c r="X9">
         <v>0.1689946024823423</v>
       </c>
-      <c r="T9">
+      <c r="Y9">
         <v>0.91528388121352955</v>
       </c>
-      <c r="U9">
+      <c r="Z9">
         <v>0.1257251558483341</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -2468,19 +3334,34 @@
         <v>1.4823518147633051E-5</v>
       </c>
       <c r="R10">
+        <v>9.4099467097041867E-5</v>
+      </c>
+      <c r="S10">
+        <v>4.1200503399473121E-2</v>
+      </c>
+      <c r="T10">
+        <v>2.3553326023995069E-4</v>
+      </c>
+      <c r="U10">
+        <v>1.0821478224620761E-7</v>
+      </c>
+      <c r="V10">
+        <v>1.237646607421539E-8</v>
+      </c>
+      <c r="W10">
         <v>0.70816577233760913</v>
       </c>
-      <c r="S10">
+      <c r="X10">
         <v>0.73844206657136002</v>
       </c>
-      <c r="T10">
+      <c r="Y10">
         <v>0.1229000515273513</v>
       </c>
-      <c r="U10">
+      <c r="Z10">
         <v>1.730939609768534E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -2530,19 +3411,34 @@
         <v>0.34934857978495598</v>
       </c>
       <c r="R11">
+        <v>1.2334535830545329E-2</v>
+      </c>
+      <c r="S11">
+        <v>1.1564976966305099E-5</v>
+      </c>
+      <c r="T11">
+        <v>6.9926977647474242E-3</v>
+      </c>
+      <c r="U11">
+        <v>6.4875767495231607E-3</v>
+      </c>
+      <c r="V11">
+        <v>0.49622031671699451</v>
+      </c>
+      <c r="W11">
         <v>2.795416367273873E-7</v>
       </c>
-      <c r="S11">
+      <c r="X11">
         <v>8.5709217501062085E-14</v>
       </c>
-      <c r="T11">
+      <c r="Y11">
         <v>0.30542350940214602</v>
       </c>
-      <c r="U11">
+      <c r="Z11">
         <v>2.2583764572559062E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -2592,19 +3488,34 @@
         <v>6.2786588008982402E-2</v>
       </c>
       <c r="R12">
+        <v>0.74743360847980478</v>
+      </c>
+      <c r="S12">
+        <v>6.1083923840136167E-2</v>
+      </c>
+      <c r="T12">
+        <v>0.7221208232459988</v>
+      </c>
+      <c r="U12">
+        <v>0.1191317184639136</v>
+      </c>
+      <c r="V12">
+        <v>0.42555768854234582</v>
+      </c>
+      <c r="W12">
         <v>8.0905576936931345E-2</v>
       </c>
-      <c r="S12">
+      <c r="X12">
         <v>4.0295991308370033E-4</v>
       </c>
-      <c r="T12">
+      <c r="Y12">
         <v>0.43187306240811002</v>
       </c>
-      <c r="U12">
+      <c r="Z12">
         <v>0.17798805987451519</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -2654,19 +3565,34 @@
         <v>0</v>
       </c>
       <c r="R13">
+        <v>2.0368010967874989E-4</v>
+      </c>
+      <c r="S13">
+        <v>0.27705992773981869</v>
+      </c>
+      <c r="T13">
+        <v>3.2434438828765622E-4</v>
+      </c>
+      <c r="U13">
+        <v>4.3626802411989019E-5</v>
+      </c>
+      <c r="V13">
+        <v>3.796236321740309E-6</v>
+      </c>
+      <c r="W13">
         <v>0.86739151382489088</v>
       </c>
-      <c r="S13">
+      <c r="X13">
         <v>5.151818129720942E-2</v>
       </c>
-      <c r="T13">
+      <c r="Y13">
         <v>3.7012783159179552E-2</v>
       </c>
-      <c r="U13">
+      <c r="Z13">
         <v>4.3311479002120727E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -2716,19 +3642,34 @@
         <v>5.4648374714361125E-10</v>
       </c>
       <c r="R14">
+        <v>3.4891757347477181E-3</v>
+      </c>
+      <c r="S14">
+        <v>0.79063531541032228</v>
+      </c>
+      <c r="T14">
+        <v>4.0410314315659779E-3</v>
+      </c>
+      <c r="U14">
+        <v>3.676623639974852E-2</v>
+      </c>
+      <c r="V14">
+        <v>6.1323783667970311E-3</v>
+      </c>
+      <c r="W14">
         <v>8.9097289615357234E-2</v>
       </c>
-      <c r="S14">
+      <c r="X14">
         <v>0.120060261890508</v>
       </c>
-      <c r="T14">
+      <c r="Y14">
         <v>0.19484935352930099</v>
       </c>
-      <c r="U14">
+      <c r="Z14">
         <v>0.1137832484616574</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -2778,19 +3719,34 @@
         <v>0</v>
       </c>
       <c r="R15">
+        <v>1.9887008817631721E-4</v>
+      </c>
+      <c r="S15">
+        <v>0.30015989643120999</v>
+      </c>
+      <c r="T15">
+        <v>3.1302547499634242E-4</v>
+      </c>
+      <c r="U15">
+        <v>5.4127560781935813E-5</v>
+      </c>
+      <c r="V15">
+        <v>4.500966554354946E-6</v>
+      </c>
+      <c r="W15">
         <v>0.80770325479877614</v>
       </c>
-      <c r="S15">
+      <c r="X15">
         <v>5.1803057332674651E-2</v>
       </c>
-      <c r="T15">
+      <c r="Y15">
         <v>3.7239775487832187E-2</v>
       </c>
-      <c r="U15">
+      <c r="Z15">
         <v>4.2086543145088529E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -2840,19 +3796,34 @@
         <v>0</v>
       </c>
       <c r="R16">
+        <v>0.68143302767301495</v>
+      </c>
+      <c r="S16">
+        <v>1.9598951843968541E-2</v>
+      </c>
+      <c r="T16">
+        <v>0.78599708555229109</v>
+      </c>
+      <c r="U16">
+        <v>5.3823453703005786E-3</v>
+      </c>
+      <c r="V16">
+        <v>2.1261774945706691E-2</v>
+      </c>
+      <c r="W16">
         <v>1.0499954647067431E-3</v>
       </c>
-      <c r="S16">
+      <c r="X16">
         <v>0.87606509519484943</v>
       </c>
-      <c r="T16">
+      <c r="Y16">
         <v>0.50971126645278453</v>
       </c>
-      <c r="U16">
+      <c r="Z16">
         <v>0.27758605659114283</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -2902,263 +3873,723 @@
         <v>0</v>
       </c>
       <c r="R17">
+        <v>4.2970223464413593E-3</v>
+      </c>
+      <c r="S17">
+        <v>5.2555385058693282E-2</v>
+      </c>
+      <c r="T17">
+        <v>7.2250466000358671E-3</v>
+      </c>
+      <c r="U17">
+        <v>2.23814495068364E-5</v>
+      </c>
+      <c r="V17">
+        <v>8.3638338521652145E-6</v>
+      </c>
+      <c r="W17">
         <v>0.14600928530801219</v>
       </c>
-      <c r="S17">
+      <c r="X17">
         <v>9.0590368050996073E-2</v>
       </c>
-      <c r="T17">
+      <c r="Y17">
         <v>9.5589031800059843E-2</v>
       </c>
-      <c r="U17">
+      <c r="Z17">
         <v>3.6711625331257158E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>1.5234122749419039E-3</v>
+      </c>
+      <c r="C18">
+        <v>0.18042785785380319</v>
+      </c>
+      <c r="D18">
+        <v>0.64276199117829647</v>
+      </c>
+      <c r="E18">
+        <v>9.7428371433279981E-2</v>
+      </c>
+      <c r="F18">
+        <v>0.2493176011176246</v>
+      </c>
+      <c r="G18">
+        <v>0.47707431191177768</v>
+      </c>
+      <c r="H18">
+        <v>1.7666464176002709E-6</v>
+      </c>
+      <c r="I18">
+        <v>1.278985204954397E-3</v>
+      </c>
+      <c r="J18">
+        <v>2.3553326023995069E-4</v>
+      </c>
+      <c r="K18">
+        <v>6.9926977647474242E-3</v>
+      </c>
+      <c r="L18">
+        <v>0.7221208232459988</v>
+      </c>
+      <c r="M18">
+        <v>3.2434438828765622E-4</v>
+      </c>
+      <c r="N18">
+        <v>4.0410314315659779E-3</v>
+      </c>
+      <c r="O18">
+        <v>3.1302547499634242E-4</v>
+      </c>
+      <c r="P18">
+        <v>0.78599708555229109</v>
+      </c>
+      <c r="Q18">
+        <v>7.2250466000358671E-3</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>3.8413716652030423E-14</v>
+      </c>
+      <c r="U18">
+        <v>5.3881343831108097E-12</v>
+      </c>
+      <c r="V18">
+        <v>0</v>
+      </c>
+      <c r="W18">
+        <v>0.81127543085422515</v>
+      </c>
+      <c r="X18">
+        <v>8.0018966353812004E-4</v>
+      </c>
+      <c r="Y18">
+        <v>0.86795693149647413</v>
+      </c>
+      <c r="Z18">
+        <v>6.6420681439741891E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B18">
-        <v>7.9940312147641635E-9</v>
-      </c>
-      <c r="C18">
-        <v>0.14201147788876761</v>
-      </c>
-      <c r="D18">
-        <v>0.22097305700749681</v>
-      </c>
-      <c r="E18">
-        <v>2.623544624303786E-2</v>
-      </c>
-      <c r="F18">
-        <v>0.12747029830778309</v>
-      </c>
-      <c r="G18">
-        <v>0.35272965857318411</v>
-      </c>
-      <c r="H18">
-        <v>0.84948185369671969</v>
-      </c>
-      <c r="I18">
-        <v>0.98317360079058647</v>
-      </c>
-      <c r="J18">
-        <v>0.70816577233760913</v>
-      </c>
-      <c r="K18">
-        <v>2.795416367273873E-7</v>
-      </c>
-      <c r="L18">
-        <v>8.0905576936931345E-2</v>
-      </c>
-      <c r="M18">
-        <v>0.86739151382489088</v>
-      </c>
-      <c r="N18">
-        <v>8.9097289615357234E-2</v>
-      </c>
-      <c r="O18">
-        <v>0.80770325479877614</v>
-      </c>
-      <c r="P18">
-        <v>1.0499954647067431E-3</v>
-      </c>
-      <c r="Q18">
-        <v>0.14600928530801219</v>
-      </c>
-      <c r="S18">
-        <v>3.0903577067360018E-2</v>
-      </c>
-      <c r="T18">
-        <v>0.90114062988461674</v>
-      </c>
-      <c r="U18">
-        <v>4.3382082287099388E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+      <c r="B19">
+        <v>3.0354181976899319E-3</v>
+      </c>
+      <c r="C19">
+        <v>0.15757841399975231</v>
+      </c>
+      <c r="D19">
+        <v>0.78426958913470668</v>
+      </c>
+      <c r="E19">
+        <v>0.1091206331934611</v>
+      </c>
+      <c r="F19">
+        <v>0.31840143037489699</v>
+      </c>
+      <c r="G19">
+        <v>0.38543230182208182</v>
+      </c>
+      <c r="H19">
+        <v>8.5552872164385008E-7</v>
+      </c>
+      <c r="I19">
+        <v>6.1382250129948801E-4</v>
+      </c>
+      <c r="J19">
+        <v>9.4099467097041867E-5</v>
+      </c>
+      <c r="K19">
+        <v>1.2334535830545329E-2</v>
+      </c>
+      <c r="L19">
+        <v>0.74743360847980478</v>
+      </c>
+      <c r="M19">
+        <v>2.0368010967874989E-4</v>
+      </c>
+      <c r="N19">
+        <v>3.4891757347477181E-3</v>
+      </c>
+      <c r="O19">
+        <v>1.9887008817631721E-4</v>
+      </c>
+      <c r="P19">
+        <v>0.68143302767301495</v>
+      </c>
+      <c r="Q19">
+        <v>4.2970223464413593E-3</v>
+      </c>
+      <c r="S19">
+        <v>2.5691448968245819E-11</v>
+      </c>
+      <c r="T19">
+        <v>0</v>
+      </c>
+      <c r="U19">
+        <v>7.5495165674510645E-15</v>
+      </c>
+      <c r="V19">
+        <v>0</v>
+      </c>
+      <c r="W19">
+        <v>0.80120129902200077</v>
+      </c>
+      <c r="X19">
+        <v>6.2083467018125837E-4</v>
+      </c>
+      <c r="Y19">
+        <v>0.91246038429099485</v>
+      </c>
+      <c r="Z19">
+        <v>6.789050827400378E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B19">
-        <v>1.5294654431841082E-11</v>
-      </c>
-      <c r="C19">
-        <v>3.4065538884172852E-2</v>
-      </c>
-      <c r="D19">
-        <v>0.81809164219173258</v>
-      </c>
-      <c r="E19">
-        <v>1.6297710362367161E-2</v>
-      </c>
-      <c r="F19">
-        <v>1.787699543953636E-9</v>
-      </c>
-      <c r="G19">
-        <v>6.9762797552677336E-2</v>
-      </c>
-      <c r="H19">
-        <v>0.1760831168296795</v>
-      </c>
-      <c r="I19">
-        <v>0.1689946024823423</v>
-      </c>
-      <c r="J19">
-        <v>0.73844206657136002</v>
-      </c>
-      <c r="K19">
-        <v>8.5709217501062085E-14</v>
-      </c>
-      <c r="L19">
-        <v>4.0295991308370033E-4</v>
-      </c>
-      <c r="M19">
-        <v>5.151818129720942E-2</v>
-      </c>
-      <c r="N19">
-        <v>0.120060261890508</v>
-      </c>
-      <c r="O19">
-        <v>5.1803057332674651E-2</v>
-      </c>
-      <c r="P19">
-        <v>0.87606509519484943</v>
-      </c>
-      <c r="Q19">
-        <v>9.0590368050996073E-2</v>
-      </c>
-      <c r="R19">
-        <v>3.0903577067360018E-2</v>
-      </c>
-      <c r="T19">
-        <v>0.42536852396805402</v>
-      </c>
-      <c r="U19">
-        <v>4.664918729635259E-3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="B20">
-        <v>0.52351544353247403</v>
+        <v>2.0223074938652269E-4</v>
       </c>
       <c r="C20">
-        <v>0.94678857817506135</v>
+        <v>0.16454747370130329</v>
       </c>
       <c r="D20">
-        <v>0.68861967565947912</v>
+        <v>4.4397665061057801E-4</v>
       </c>
       <c r="E20">
-        <v>0.67751416115935603</v>
+        <v>0.19393981618976919</v>
       </c>
       <c r="F20">
-        <v>0.79170857727050126</v>
+        <v>1.3027048439997471E-3</v>
       </c>
       <c r="G20">
-        <v>0.50292835471340336</v>
+        <v>3.8318701261943033E-2</v>
       </c>
       <c r="H20">
-        <v>4.2688932613786923E-2</v>
+        <v>0.43191446071589651</v>
       </c>
       <c r="I20">
-        <v>0.91528388121352955</v>
+        <v>3.8516460401481822E-2</v>
       </c>
       <c r="J20">
-        <v>0.1229000515273513</v>
+        <v>4.1200503399473121E-2</v>
       </c>
       <c r="K20">
-        <v>0.30542350940214602</v>
+        <v>1.1564976966305099E-5</v>
       </c>
       <c r="L20">
-        <v>0.43187306240811002</v>
+        <v>6.1083923840136167E-2</v>
       </c>
       <c r="M20">
-        <v>3.7012783159179552E-2</v>
+        <v>0.27705992773981869</v>
       </c>
       <c r="N20">
-        <v>0.19484935352930099</v>
+        <v>0.79063531541032228</v>
       </c>
       <c r="O20">
-        <v>3.7239775487832187E-2</v>
+        <v>0.30015989643120999</v>
       </c>
       <c r="P20">
-        <v>0.50971126645278453</v>
+        <v>1.9598951843968541E-2</v>
       </c>
       <c r="Q20">
-        <v>9.5589031800059843E-2</v>
+        <v>5.2555385058693282E-2</v>
       </c>
       <c r="R20">
-        <v>0.90114062988461674</v>
-      </c>
-      <c r="S20">
-        <v>0.42536852396805402</v>
+        <v>2.5691448968245819E-11</v>
+      </c>
+      <c r="T20">
+        <v>3.8413716652030423E-14</v>
       </c>
       <c r="U20">
-        <v>2.0071152893850201E-3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="V20">
+        <v>3.415871683287719E-7</v>
+      </c>
+      <c r="W20">
+        <v>0.27242866578011582</v>
+      </c>
+      <c r="X20">
+        <v>0.69770597861268868</v>
+      </c>
+      <c r="Y20">
+        <v>0.4531724772561696</v>
+      </c>
+      <c r="Z20">
+        <v>0.70913788899827823</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B21">
+        <v>8.2416198412975872E-2</v>
+      </c>
+      <c r="C21">
+        <v>1.8746157816013301E-2</v>
+      </c>
+      <c r="D21">
+        <v>2.3377543571192478E-3</v>
+      </c>
+      <c r="E21">
+        <v>0.90776054857610999</v>
+      </c>
+      <c r="F21">
+        <v>2.4634913323675619E-2</v>
+      </c>
+      <c r="G21">
+        <v>5.7583542686199252E-3</v>
+      </c>
+      <c r="H21">
+        <v>2.0138057497121049E-6</v>
+      </c>
+      <c r="I21">
+        <v>2.156992431334714E-6</v>
+      </c>
+      <c r="J21">
+        <v>1.0821478224620761E-7</v>
+      </c>
+      <c r="K21">
+        <v>6.4875767495231607E-3</v>
+      </c>
+      <c r="L21">
+        <v>0.1191317184639136</v>
+      </c>
+      <c r="M21">
+        <v>4.3626802411989019E-5</v>
+      </c>
+      <c r="N21">
+        <v>3.676623639974852E-2</v>
+      </c>
+      <c r="O21">
+        <v>5.4127560781935813E-5</v>
+      </c>
+      <c r="P21">
+        <v>5.3823453703005786E-3</v>
+      </c>
+      <c r="Q21">
+        <v>2.23814495068364E-5</v>
+      </c>
+      <c r="R21">
+        <v>7.5495165674510645E-15</v>
+      </c>
+      <c r="S21">
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <v>5.3881343831108097E-12</v>
+      </c>
+      <c r="V21">
+        <v>0</v>
+      </c>
+      <c r="W21">
+        <v>0.78098984192134679</v>
+      </c>
+      <c r="X21">
+        <v>6.7511970787562658E-2</v>
+      </c>
+      <c r="Y21">
+        <v>0.56386775023430746</v>
+      </c>
+      <c r="Z21">
+        <v>0.41598709377972543</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>0.91507425958794109</v>
+      </c>
+      <c r="C22">
+        <v>1.9877306910976111E-2</v>
+      </c>
+      <c r="D22">
+        <v>4.374825080269451E-2</v>
+      </c>
+      <c r="E22">
+        <v>0.50529511325417786</v>
+      </c>
+      <c r="F22">
+        <v>0.35205785424784031</v>
+      </c>
+      <c r="G22">
+        <v>1.3491751282044721E-2</v>
+      </c>
+      <c r="H22">
+        <v>8.2320865679719191E-9</v>
+      </c>
+      <c r="I22">
+        <v>4.4866565440671019E-7</v>
+      </c>
+      <c r="J22">
+        <v>1.237646607421539E-8</v>
+      </c>
+      <c r="K22">
+        <v>0.49622031671699451</v>
+      </c>
+      <c r="L22">
+        <v>0.42555768854234582</v>
+      </c>
+      <c r="M22">
+        <v>3.796236321740309E-6</v>
+      </c>
+      <c r="N22">
+        <v>6.1323783667970311E-3</v>
+      </c>
+      <c r="O22">
+        <v>4.500966554354946E-6</v>
+      </c>
+      <c r="P22">
+        <v>2.1261774945706691E-2</v>
+      </c>
+      <c r="Q22">
+        <v>8.3638338521652145E-6</v>
+      </c>
+      <c r="R22">
+        <v>0</v>
+      </c>
+      <c r="S22">
+        <v>3.415871683287719E-7</v>
+      </c>
+      <c r="T22">
+        <v>0</v>
+      </c>
+      <c r="U22">
+        <v>0</v>
+      </c>
+      <c r="W22">
+        <v>0.80087581500474503</v>
+      </c>
+      <c r="X22">
+        <v>3.3129503630568991E-3</v>
+      </c>
+      <c r="Y22">
+        <v>0.77285325956540563</v>
+      </c>
+      <c r="Z22">
+        <v>0.16024733528434559</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>7.9940312147641635E-9</v>
+      </c>
+      <c r="C23">
+        <v>0.14201147788876761</v>
+      </c>
+      <c r="D23">
+        <v>0.22097305700749681</v>
+      </c>
+      <c r="E23">
+        <v>2.623544624303786E-2</v>
+      </c>
+      <c r="F23">
+        <v>0.12747029830778309</v>
+      </c>
+      <c r="G23">
+        <v>0.35272965857318411</v>
+      </c>
+      <c r="H23">
+        <v>0.84948185369671969</v>
+      </c>
+      <c r="I23">
+        <v>0.98317360079058647</v>
+      </c>
+      <c r="J23">
+        <v>0.70816577233760913</v>
+      </c>
+      <c r="K23">
+        <v>2.795416367273873E-7</v>
+      </c>
+      <c r="L23">
+        <v>8.0905576936931345E-2</v>
+      </c>
+      <c r="M23">
+        <v>0.86739151382489088</v>
+      </c>
+      <c r="N23">
+        <v>8.9097289615357234E-2</v>
+      </c>
+      <c r="O23">
+        <v>0.80770325479877614</v>
+      </c>
+      <c r="P23">
+        <v>1.0499954647067431E-3</v>
+      </c>
+      <c r="Q23">
+        <v>0.14600928530801219</v>
+      </c>
+      <c r="R23">
+        <v>0.80120129902200077</v>
+      </c>
+      <c r="S23">
+        <v>0.27242866578011582</v>
+      </c>
+      <c r="T23">
+        <v>0.81127543085422515</v>
+      </c>
+      <c r="U23">
+        <v>0.78098984192134679</v>
+      </c>
+      <c r="V23">
+        <v>0.80087581500474503</v>
+      </c>
+      <c r="X23">
+        <v>3.0903577067360018E-2</v>
+      </c>
+      <c r="Y23">
+        <v>0.90114062988461674</v>
+      </c>
+      <c r="Z23">
+        <v>4.3382082287099388E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>1.5294654431841082E-11</v>
+      </c>
+      <c r="C24">
+        <v>3.4065538884172852E-2</v>
+      </c>
+      <c r="D24">
+        <v>0.81809164219173258</v>
+      </c>
+      <c r="E24">
+        <v>1.6297710362367161E-2</v>
+      </c>
+      <c r="F24">
+        <v>1.787699543953636E-9</v>
+      </c>
+      <c r="G24">
+        <v>6.9762797552677336E-2</v>
+      </c>
+      <c r="H24">
+        <v>0.1760831168296795</v>
+      </c>
+      <c r="I24">
+        <v>0.1689946024823423</v>
+      </c>
+      <c r="J24">
+        <v>0.73844206657136002</v>
+      </c>
+      <c r="K24">
+        <v>8.5709217501062085E-14</v>
+      </c>
+      <c r="L24">
+        <v>4.0295991308370033E-4</v>
+      </c>
+      <c r="M24">
+        <v>5.151818129720942E-2</v>
+      </c>
+      <c r="N24">
+        <v>0.120060261890508</v>
+      </c>
+      <c r="O24">
+        <v>5.1803057332674651E-2</v>
+      </c>
+      <c r="P24">
+        <v>0.87606509519484943</v>
+      </c>
+      <c r="Q24">
+        <v>9.0590368050996073E-2</v>
+      </c>
+      <c r="R24">
+        <v>6.2083467018125837E-4</v>
+      </c>
+      <c r="S24">
+        <v>0.69770597861268868</v>
+      </c>
+      <c r="T24">
+        <v>8.0018966353812004E-4</v>
+      </c>
+      <c r="U24">
+        <v>6.7511970787562658E-2</v>
+      </c>
+      <c r="V24">
+        <v>3.3129503630568991E-3</v>
+      </c>
+      <c r="W24">
+        <v>3.0903577067360018E-2</v>
+      </c>
+      <c r="Y24">
+        <v>0.42536852396805402</v>
+      </c>
+      <c r="Z24">
+        <v>4.664918729635259E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>0.52351544353247403</v>
+      </c>
+      <c r="C25">
+        <v>0.94678857817506135</v>
+      </c>
+      <c r="D25">
+        <v>0.68861967565947912</v>
+      </c>
+      <c r="E25">
+        <v>0.67751416115935603</v>
+      </c>
+      <c r="F25">
+        <v>0.79170857727050126</v>
+      </c>
+      <c r="G25">
+        <v>0.50292835471340336</v>
+      </c>
+      <c r="H25">
+        <v>4.2688932613786923E-2</v>
+      </c>
+      <c r="I25">
+        <v>0.91528388121352955</v>
+      </c>
+      <c r="J25">
+        <v>0.1229000515273513</v>
+      </c>
+      <c r="K25">
+        <v>0.30542350940214602</v>
+      </c>
+      <c r="L25">
+        <v>0.43187306240811002</v>
+      </c>
+      <c r="M25">
+        <v>3.7012783159179552E-2</v>
+      </c>
+      <c r="N25">
+        <v>0.19484935352930099</v>
+      </c>
+      <c r="O25">
+        <v>3.7239775487832187E-2</v>
+      </c>
+      <c r="P25">
+        <v>0.50971126645278453</v>
+      </c>
+      <c r="Q25">
+        <v>9.5589031800059843E-2</v>
+      </c>
+      <c r="R25">
+        <v>0.91246038429099485</v>
+      </c>
+      <c r="S25">
+        <v>0.4531724772561696</v>
+      </c>
+      <c r="T25">
+        <v>0.86795693149647413</v>
+      </c>
+      <c r="U25">
+        <v>0.56386775023430746</v>
+      </c>
+      <c r="V25">
+        <v>0.77285325956540563</v>
+      </c>
+      <c r="W25">
+        <v>0.90114062988461674</v>
+      </c>
+      <c r="X25">
+        <v>0.42536852396805402</v>
+      </c>
+      <c r="Z25">
+        <v>2.0071152893850201E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26">
         <v>1.9855965758854839E-3</v>
       </c>
-      <c r="C21">
+      <c r="C26">
         <v>0.11197844587601311</v>
       </c>
-      <c r="D21">
+      <c r="D26">
         <v>0.32843522518317952</v>
       </c>
-      <c r="E21">
+      <c r="E26">
         <v>0.20483667461513291</v>
       </c>
-      <c r="F21">
+      <c r="F26">
         <v>7.884574595334648E-3</v>
       </c>
-      <c r="G21">
+      <c r="G26">
         <v>0.19660505964039571</v>
       </c>
-      <c r="H21">
+      <c r="H26">
         <v>0.49437267771767651</v>
       </c>
-      <c r="I21">
+      <c r="I26">
         <v>0.1257251558483341</v>
       </c>
-      <c r="J21">
+      <c r="J26">
         <v>1.730939609768534E-2</v>
       </c>
-      <c r="K21">
+      <c r="K26">
         <v>2.2583764572559062E-3</v>
       </c>
-      <c r="L21">
+      <c r="L26">
         <v>0.17798805987451519</v>
       </c>
-      <c r="M21">
+      <c r="M26">
         <v>4.3311479002120727E-2</v>
       </c>
-      <c r="N21">
+      <c r="N26">
         <v>0.1137832484616574</v>
       </c>
-      <c r="O21">
+      <c r="O26">
         <v>4.2086543145088529E-2</v>
       </c>
-      <c r="P21">
+      <c r="P26">
         <v>0.27758605659114283</v>
       </c>
-      <c r="Q21">
+      <c r="Q26">
         <v>3.6711625331257158E-2</v>
       </c>
-      <c r="R21">
+      <c r="R26">
+        <v>6.789050827400378E-2</v>
+      </c>
+      <c r="S26">
+        <v>0.70913788899827823</v>
+      </c>
+      <c r="T26">
+        <v>6.6420681439741891E-2</v>
+      </c>
+      <c r="U26">
+        <v>0.41598709377972543</v>
+      </c>
+      <c r="V26">
+        <v>0.16024733528434559</v>
+      </c>
+      <c r="W26">
         <v>4.3382082287099388E-2</v>
       </c>
-      <c r="S21">
+      <c r="X26">
         <v>4.664918729635259E-3</v>
       </c>
-      <c r="T21">
+      <c r="Y26">
         <v>2.0071152893850201E-3</v>
       </c>
     </row>

</xml_diff>